<commit_message>
parallelStream has a limit on cores (default is 16 because of hyper-threading)
</commit_message>
<xml_diff>
--- a/Task_2_1_1/graphs.xlsx
+++ b/Task_2_1_1/graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mi\Desktop\vuz proga\nsujava\Task_2_1_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FB5F5A-61D4-4A29-AB26-725419A8AB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C32C85-AD00-4A5F-8884-87CA2E361E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14746" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Single</t>
   </si>
   <si>
-    <t>PS</t>
+    <t>Multi (8 cores)</t>
   </si>
   <si>
-    <t>Multi (8 cores)</t>
+    <t>PS (8 cores)</t>
+  </si>
+  <si>
+    <t>Multi (6 cores)</t>
+  </si>
+  <si>
+    <t>PS (6 cores)</t>
   </si>
 </sst>
 </file>
@@ -121,6 +127,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi (8 cores)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -171,7 +188,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$2:$I$2</c:f>
+              <c:f>Лист1!$A$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -194,13 +211,13 @@
                   <c:v>3839</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5763</c:v>
+                  <c:v>5310</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7375</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9812</c:v>
+                  <c:v>9250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -215,6 +232,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Single</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -265,7 +293,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$A$3:$I$3</c:f>
+              <c:f>Лист1!$A$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -309,6 +337,17 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PS (8 cores)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -364,31 +403,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227</c:v>
+                  <c:v>173</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3951</c:v>
+                  <c:v>994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8471</c:v>
+                  <c:v>1998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16481</c:v>
+                  <c:v>3901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23328</c:v>
+                  <c:v>5541</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30893</c:v>
+                  <c:v>7744</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42209</c:v>
+                  <c:v>9393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -397,6 +436,144 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0A21-4863-B86C-5002BBBB85FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Multi (6 cores)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$A$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1020</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1786</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3581</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6956</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8747</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-36FD-4525-8222-9C115D475319}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$J$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PS (6 cores)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$A$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>948</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1872</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3768</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5479</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7415</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9289</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-36FD-4525-8222-9C115D475319}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1131,16 +1308,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1431,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1473,98 +1650,162 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
         <v>56</v>
       </c>
-      <c r="B2">
-        <v>71</v>
-      </c>
       <c r="C2">
-        <v>310</v>
+        <v>670</v>
       </c>
       <c r="D2">
-        <v>915</v>
+        <v>4828</v>
       </c>
       <c r="E2">
-        <v>2036</v>
+        <v>9528</v>
       </c>
       <c r="F2">
-        <v>3839</v>
+        <v>19062</v>
       </c>
       <c r="G2">
-        <v>5763</v>
+        <v>28588</v>
       </c>
       <c r="H2">
-        <v>7375</v>
+        <v>38107</v>
       </c>
       <c r="I2">
-        <v>9812</v>
+        <v>47620</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>670</v>
+        <v>310</v>
       </c>
       <c r="D3">
-        <v>4828</v>
+        <v>915</v>
       </c>
       <c r="E3">
-        <v>9528</v>
+        <v>2036</v>
       </c>
       <c r="F3">
-        <v>19062</v>
+        <v>3839</v>
       </c>
       <c r="G3">
-        <v>28588</v>
+        <v>5310</v>
       </c>
       <c r="H3">
-        <v>38107</v>
+        <v>7375</v>
       </c>
       <c r="I3">
-        <v>47620</v>
+        <v>9250</v>
       </c>
       <c r="J3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B4">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>227</v>
+        <v>173</v>
       </c>
       <c r="D4">
-        <v>3951</v>
+        <v>994</v>
       </c>
       <c r="E4">
-        <v>8471</v>
+        <v>1998</v>
       </c>
       <c r="F4">
-        <v>16481</v>
+        <v>3901</v>
       </c>
       <c r="G4">
-        <v>23328</v>
+        <v>5541</v>
       </c>
       <c r="H4">
-        <v>30893</v>
+        <v>7744</v>
       </c>
       <c r="I4">
-        <v>42209</v>
+        <v>9393</v>
       </c>
       <c r="J4" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>191</v>
+      </c>
+      <c r="D5">
+        <v>1020</v>
+      </c>
+      <c r="E5">
+        <v>1786</v>
+      </c>
+      <c r="F5">
+        <v>3581</v>
+      </c>
+      <c r="G5">
+        <v>5145</v>
+      </c>
+      <c r="H5">
+        <v>6956</v>
+      </c>
+      <c r="I5">
+        <v>8747</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>120</v>
+      </c>
+      <c r="D6">
+        <v>948</v>
+      </c>
+      <c r="E6">
+        <v>1872</v>
+      </c>
+      <c r="F6">
+        <v>3768</v>
+      </c>
+      <c r="G6">
+        <v>5479</v>
+      </c>
+      <c r="H6">
+        <v>7415</v>
+      </c>
+      <c r="I6">
+        <v>9289</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>